<commit_message>
Correct 0201 capacitor footprint to 0603,  correct 470kohms resistor for supply reason
</commit_message>
<xml_diff>
--- a/SMD capacitor kits/smd_capacitor kit.xlsx
+++ b/SMD capacitor kits/smd_capacitor kit.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raphael\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taula\Desktop\Swissairtainer\BOM\Orderable_components\SMD capacitor kits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997F7038-39E7-4C79-BCFE-9B5AC29BAFD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1895FC5-9FEE-4409-9A58-EF6D1852D8A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-8700" windowWidth="29040" windowHeight="17520" xr2:uid="{15C58183-1DDA-4A24-B1F3-2EB92C9813C1}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{15C58183-1DDA-4A24-B1F3-2EB92C9813C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -194,18 +194,6 @@
     <t>603-CC603JRX7R7BB224</t>
   </si>
   <si>
-    <t>581-02013A220FAT2A</t>
-  </si>
-  <si>
-    <t>02013A220FAT2A</t>
-  </si>
-  <si>
-    <t>791-0201N101J250CT</t>
-  </si>
-  <si>
-    <t>0201N101J250CT</t>
-  </si>
-  <si>
     <t>187-CL21C101JBANNNC</t>
   </si>
   <si>
@@ -240,6 +228,18 @@
   </si>
   <si>
     <t>10</t>
+  </si>
+  <si>
+    <t>603-AC603JRNPO9BN220</t>
+  </si>
+  <si>
+    <t>AC0603JRNPO9BN220</t>
+  </si>
+  <si>
+    <t>791-0603N101J160CT</t>
+  </si>
+  <si>
+    <t>0603N101J160CT</t>
   </si>
 </sst>
 </file>
@@ -287,10 +287,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -310,7 +309,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -609,20 +608,20 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="1"/>
-    <col min="2" max="2" width="12.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1328125" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="23" style="1" customWidth="1"/>
-    <col min="5" max="6" width="25.109375" style="1" customWidth="1"/>
+    <col min="5" max="6" width="25.1328125" style="1" customWidth="1"/>
     <col min="7" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -633,15 +632,15 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -656,9 +655,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
@@ -673,9 +672,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -690,9 +689,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
@@ -707,26 +706,26 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
@@ -741,9 +740,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>6</v>
@@ -752,15 +751,15 @@
         <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
@@ -775,9 +774,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
@@ -786,15 +785,15 @@
         <v>15</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
@@ -803,15 +802,15 @@
         <v>16</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>8</v>
@@ -820,15 +819,15 @@
         <v>15</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>8</v>
@@ -837,15 +836,15 @@
         <v>16</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>9</v>
@@ -860,9 +859,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>9</v>
@@ -877,9 +876,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>10</v>
@@ -894,9 +893,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>10</v>
@@ -911,9 +910,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>11</v>
@@ -928,9 +927,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>11</v>
@@ -945,12 +944,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>15</v>
@@ -962,9 +961,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>12</v>
@@ -979,9 +978,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>13</v>
@@ -996,9 +995,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>13</v>
@@ -1013,9 +1012,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>14</v>
@@ -1030,9 +1029,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>14</v>

</xml_diff>